<commit_message>
Adding work on datasets and models
</commit_message>
<xml_diff>
--- a/tables/2021AP.xlsx
+++ b/tables/2021AP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eanma\Google Drive\Data Projects\top25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eanma\Google Drive\Data Projects\top25\top25_project\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596C0663-1EB4-4970-B836-C16347E80933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9866B3E6-4B7F-4A16-B092-849DF3609D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{6BD16A16-E195-4F8C-BD1A-E4B6BB240C1C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="57">
   <si>
     <t>Team</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>Wake Forest</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>SMU</t>
+  </si>
+  <si>
+    <t>San Diego State</t>
   </si>
 </sst>
 </file>
@@ -547,11 +556,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48743F2A-DB94-4EE1-849C-517D3A883C44}">
-  <dimension ref="A1:O127"/>
+  <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="Q121" sqref="Q121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3862,7 +3871,7 @@
         <v>17</v>
       </c>
       <c r="O67">
-        <f t="shared" ref="O67:O101" si="4">C67-N67</f>
+        <f t="shared" ref="O67:O130" si="4">C67-N67</f>
         <v>-1</v>
       </c>
     </row>
@@ -3988,7 +3997,7 @@
         <v>27</v>
       </c>
       <c r="M70">
-        <f t="shared" ref="M70:M101" si="6">K70-L70</f>
+        <f t="shared" ref="M70:M126" si="6">K70-L70</f>
         <v>-10</v>
       </c>
       <c r="N70">
@@ -5053,7 +5062,7 @@
         <v>0</v>
       </c>
       <c r="F92">
-        <f t="shared" ref="F92:F126" si="8">D92/(D92+E92)</f>
+        <f t="shared" ref="F92:F151" si="8">D92/(D92+E92)</f>
         <v>1</v>
       </c>
       <c r="G92">
@@ -5565,6 +5574,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G102">
+        <v>12</v>
+      </c>
+      <c r="H102">
+        <v>1</v>
+      </c>
+      <c r="I102">
+        <v>1</v>
+      </c>
+      <c r="J102" t="s">
+        <v>31</v>
+      </c>
+      <c r="K102">
+        <v>42</v>
+      </c>
+      <c r="L102">
+        <v>21</v>
+      </c>
+      <c r="M102">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="N102">
+        <v>1</v>
+      </c>
+      <c r="O102">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
@@ -5586,6 +5624,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G103">
+        <v>8</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="I103">
+        <v>1</v>
+      </c>
+      <c r="J103" t="s">
+        <v>31</v>
+      </c>
+      <c r="K103">
+        <v>37</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103">
+        <f t="shared" si="6"/>
+        <v>37</v>
+      </c>
+      <c r="N103">
+        <v>2</v>
+      </c>
+      <c r="O103">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
@@ -5607,6 +5674,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G104">
+        <v>26</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104" t="s">
+        <v>32</v>
+      </c>
+      <c r="K104">
+        <v>24</v>
+      </c>
+      <c r="L104">
+        <v>31</v>
+      </c>
+      <c r="M104">
+        <f t="shared" si="6"/>
+        <v>-7</v>
+      </c>
+      <c r="N104">
+        <v>8</v>
+      </c>
+      <c r="O104">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
@@ -5629,6 +5725,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G105">
+        <v>26</v>
+      </c>
+      <c r="H105">
+        <v>1</v>
+      </c>
+      <c r="I105">
+        <v>1</v>
+      </c>
+      <c r="J105" t="s">
+        <v>31</v>
+      </c>
+      <c r="K105">
+        <v>24</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="N105">
+        <v>4</v>
+      </c>
+      <c r="O105">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
@@ -5651,6 +5776,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G106">
+        <v>26</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106" t="s">
+        <v>31</v>
+      </c>
+      <c r="K106">
+        <v>51</v>
+      </c>
+      <c r="L106">
+        <v>14</v>
+      </c>
+      <c r="M106">
+        <f t="shared" si="6"/>
+        <v>37</v>
+      </c>
+      <c r="N106">
+        <v>3</v>
+      </c>
+      <c r="O106">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
@@ -5673,6 +5827,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G107">
+        <v>26</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107" t="s">
+        <v>31</v>
+      </c>
+      <c r="K107">
+        <v>37</v>
+      </c>
+      <c r="L107">
+        <v>31</v>
+      </c>
+      <c r="M107">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="N107">
+        <v>6</v>
+      </c>
+      <c r="O107">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
@@ -5695,6 +5878,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G108">
+        <v>9</v>
+      </c>
+      <c r="H108">
+        <v>1</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108" t="s">
+        <v>31</v>
+      </c>
+      <c r="K108">
+        <v>24</v>
+      </c>
+      <c r="L108">
+        <v>13</v>
+      </c>
+      <c r="M108">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="N108">
+        <v>5</v>
+      </c>
+      <c r="O108">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
@@ -5717,6 +5929,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G109">
+        <v>2</v>
+      </c>
+      <c r="H109">
+        <v>1</v>
+      </c>
+      <c r="I109">
+        <v>0</v>
+      </c>
+      <c r="J109" t="s">
+        <v>32</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>37</v>
+      </c>
+      <c r="M109">
+        <f t="shared" si="6"/>
+        <v>-37</v>
+      </c>
+      <c r="N109">
+        <v>13</v>
+      </c>
+      <c r="O109">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
@@ -5739,6 +5980,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G110">
+        <v>7</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110">
+        <v>1</v>
+      </c>
+      <c r="J110" t="s">
+        <v>32</v>
+      </c>
+      <c r="K110">
+        <v>13</v>
+      </c>
+      <c r="L110">
+        <v>24</v>
+      </c>
+      <c r="M110">
+        <f t="shared" si="6"/>
+        <v>-11</v>
+      </c>
+      <c r="N110">
+        <v>14</v>
+      </c>
+      <c r="O110">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
@@ -5761,6 +6031,35 @@
         <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
+      <c r="G111">
+        <v>26</v>
+      </c>
+      <c r="H111">
+        <v>1</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111" t="s">
+        <v>32</v>
+      </c>
+      <c r="K111">
+        <v>13</v>
+      </c>
+      <c r="L111">
+        <v>20</v>
+      </c>
+      <c r="M111">
+        <f t="shared" si="6"/>
+        <v>-7</v>
+      </c>
+      <c r="N111">
+        <v>20</v>
+      </c>
+      <c r="O111">
+        <f t="shared" si="4"/>
+        <v>-10</v>
+      </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
@@ -5783,6 +6082,35 @@
         <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
+      <c r="G112">
+        <v>26</v>
+      </c>
+      <c r="H112">
+        <v>1</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112" t="s">
+        <v>31</v>
+      </c>
+      <c r="K112">
+        <v>52</v>
+      </c>
+      <c r="L112">
+        <v>13</v>
+      </c>
+      <c r="M112">
+        <f t="shared" si="6"/>
+        <v>39</v>
+      </c>
+      <c r="N112">
+        <v>7</v>
+      </c>
+      <c r="O112">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
@@ -5805,6 +6133,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G113">
+        <v>1</v>
+      </c>
+      <c r="H113">
+        <v>1</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113" t="s">
+        <v>32</v>
+      </c>
+      <c r="K113">
+        <v>21</v>
+      </c>
+      <c r="L113">
+        <v>42</v>
+      </c>
+      <c r="M113">
+        <f t="shared" si="6"/>
+        <v>-21</v>
+      </c>
+      <c r="N113">
+        <v>17</v>
+      </c>
+      <c r="O113">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
@@ -5827,6 +6184,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G114">
+        <v>26</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="J114" t="s">
+        <v>31</v>
+      </c>
+      <c r="K114">
+        <v>34</v>
+      </c>
+      <c r="L114">
+        <v>20</v>
+      </c>
+      <c r="M114">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="N114">
+        <v>10</v>
+      </c>
+      <c r="O114">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
@@ -5849,6 +6235,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G115">
+        <v>26</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115" t="s">
+        <v>31</v>
+      </c>
+      <c r="K115">
+        <v>38</v>
+      </c>
+      <c r="L115">
+        <v>17</v>
+      </c>
+      <c r="M115">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="N115">
+        <v>9</v>
+      </c>
+      <c r="O115">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
@@ -5871,6 +6286,35 @@
         <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
+      <c r="G116">
+        <v>26</v>
+      </c>
+      <c r="H116">
+        <v>1</v>
+      </c>
+      <c r="I116">
+        <v>1</v>
+      </c>
+      <c r="J116" t="s">
+        <v>32</v>
+      </c>
+      <c r="K116">
+        <v>22</v>
+      </c>
+      <c r="L116">
+        <v>26</v>
+      </c>
+      <c r="M116">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="N116">
+        <v>26</v>
+      </c>
+      <c r="O116">
+        <f t="shared" si="4"/>
+        <v>-11</v>
+      </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
@@ -5893,6 +6337,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G117">
+        <v>26</v>
+      </c>
+      <c r="H117">
+        <v>0</v>
+      </c>
+      <c r="I117">
+        <v>1</v>
+      </c>
+      <c r="J117" t="s">
+        <v>31</v>
+      </c>
+      <c r="K117">
+        <v>59</v>
+      </c>
+      <c r="L117">
+        <v>6</v>
+      </c>
+      <c r="M117">
+        <f t="shared" si="6"/>
+        <v>53</v>
+      </c>
+      <c r="N117">
+        <v>15</v>
+      </c>
+      <c r="O117">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
@@ -5915,6 +6388,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G118">
+        <v>26</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="I118">
+        <v>1</v>
+      </c>
+      <c r="J118" t="s">
+        <v>31</v>
+      </c>
+      <c r="K118">
+        <v>48</v>
+      </c>
+      <c r="L118">
+        <v>31</v>
+      </c>
+      <c r="M118">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="N118">
+        <v>11</v>
+      </c>
+      <c r="O118">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
@@ -5937,6 +6439,35 @@
         <f t="shared" si="8"/>
         <v>0.8</v>
       </c>
+      <c r="G119">
+        <v>26</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119" t="s">
+        <v>32</v>
+      </c>
+      <c r="K119">
+        <v>24</v>
+      </c>
+      <c r="L119">
+        <v>27</v>
+      </c>
+      <c r="M119">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="N119">
+        <v>26</v>
+      </c>
+      <c r="O119">
+        <f t="shared" si="4"/>
+        <v>-8</v>
+      </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
@@ -5959,6 +6490,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G120">
+        <v>21</v>
+      </c>
+      <c r="H120">
+        <v>1</v>
+      </c>
+      <c r="I120">
+        <v>1</v>
+      </c>
+      <c r="J120" t="s">
+        <v>31</v>
+      </c>
+      <c r="K120">
+        <v>17</v>
+      </c>
+      <c r="L120">
+        <v>14</v>
+      </c>
+      <c r="M120">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="N120">
+        <v>12</v>
+      </c>
+      <c r="O120">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
@@ -5981,6 +6541,35 @@
         <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
+      <c r="G121">
+        <v>26</v>
+      </c>
+      <c r="H121">
+        <v>1</v>
+      </c>
+      <c r="I121">
+        <v>1</v>
+      </c>
+      <c r="J121" t="s">
+        <v>32</v>
+      </c>
+      <c r="K121">
+        <v>23</v>
+      </c>
+      <c r="L121">
+        <v>42</v>
+      </c>
+      <c r="M121">
+        <f t="shared" si="6"/>
+        <v>-19</v>
+      </c>
+      <c r="N121">
+        <v>26</v>
+      </c>
+      <c r="O121">
+        <f t="shared" si="4"/>
+        <v>-6</v>
+      </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
@@ -6003,6 +6592,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G122">
+        <v>19</v>
+      </c>
+      <c r="H122">
+        <v>1</v>
+      </c>
+      <c r="I122">
+        <v>0</v>
+      </c>
+      <c r="J122" t="s">
+        <v>32</v>
+      </c>
+      <c r="K122">
+        <v>14</v>
+      </c>
+      <c r="L122">
+        <v>17</v>
+      </c>
+      <c r="M122">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="N122">
+        <v>26</v>
+      </c>
+      <c r="O122">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
@@ -6025,6 +6643,35 @@
         <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
+      <c r="G123">
+        <v>26</v>
+      </c>
+      <c r="H123">
+        <v>1</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123" t="s">
+        <v>31</v>
+      </c>
+      <c r="K123">
+        <v>24</v>
+      </c>
+      <c r="L123">
+        <v>19</v>
+      </c>
+      <c r="M123">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="N123">
+        <v>18</v>
+      </c>
+      <c r="O123">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
@@ -6047,6 +6694,35 @@
         <f t="shared" si="8"/>
         <v>0.75</v>
       </c>
+      <c r="G124">
+        <v>26</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>1</v>
+      </c>
+      <c r="J124" t="s">
+        <v>31</v>
+      </c>
+      <c r="K124">
+        <v>34</v>
+      </c>
+      <c r="L124">
+        <v>27</v>
+      </c>
+      <c r="M124">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="N124">
+        <v>23</v>
+      </c>
+      <c r="O124">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
@@ -6069,6 +6745,35 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
+      <c r="G125">
+        <v>26</v>
+      </c>
+      <c r="H125">
+        <v>1</v>
+      </c>
+      <c r="I125">
+        <v>1</v>
+      </c>
+      <c r="J125" t="s">
+        <v>31</v>
+      </c>
+      <c r="K125">
+        <v>37</v>
+      </c>
+      <c r="L125">
+        <v>34</v>
+      </c>
+      <c r="M125">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="N125">
+        <v>19</v>
+      </c>
+      <c r="O125">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
@@ -6091,51 +6796,629 @@
         <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
+      <c r="G126">
+        <v>26</v>
+      </c>
+      <c r="H126">
+        <v>1</v>
+      </c>
+      <c r="I126">
+        <v>1</v>
+      </c>
+      <c r="J126" t="s">
+        <v>31</v>
+      </c>
+      <c r="K126">
+        <v>19</v>
+      </c>
+      <c r="L126">
+        <v>13</v>
+      </c>
+      <c r="M126">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="N126">
+        <v>26</v>
+      </c>
+      <c r="O126">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>0</v>
-      </c>
-      <c r="B127" t="s">
+        <v>1</v>
+      </c>
+      <c r="B127">
+        <v>6</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>5</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>5</v>
+      </c>
+      <c r="B128">
+        <v>6</v>
+      </c>
+      <c r="C128">
+        <f>C127+1</f>
+        <v>2</v>
+      </c>
+      <c r="D128">
+        <v>5</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>35</v>
+      </c>
+      <c r="B129">
+        <v>6</v>
+      </c>
+      <c r="C129">
+        <f t="shared" ref="C129:C151" si="10">C128+1</f>
+        <v>3</v>
+      </c>
+      <c r="D129">
+        <v>5</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>18</v>
+      </c>
+      <c r="B130">
+        <v>6</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="D130">
+        <v>5</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>8</v>
+      </c>
+      <c r="B131">
+        <v>6</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="D131">
+        <v>4</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132">
+        <v>6</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="D132">
+        <v>5</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133">
+        <v>6</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="D133">
+        <v>4</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>11</v>
+      </c>
+      <c r="B134">
+        <v>6</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="D134">
+        <v>4</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>44</v>
+      </c>
+      <c r="B135">
+        <v>6</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="D135">
+        <v>5</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>43</v>
+      </c>
+      <c r="B136">
+        <v>6</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="D136">
+        <v>5</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>47</v>
+      </c>
+      <c r="B137">
+        <v>6</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="D137">
+        <v>5</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>50</v>
+      </c>
+      <c r="B138">
+        <v>6</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="D138">
+        <v>5</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>42</v>
+      </c>
+      <c r="B139">
+        <v>6</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="D139">
+        <v>4</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>9</v>
+      </c>
+      <c r="B140">
+        <v>6</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="D140">
+        <v>4</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>21</v>
+      </c>
+      <c r="B141">
+        <v>6</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="D141">
+        <v>5</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>54</v>
+      </c>
+      <c r="B142">
+        <v>6</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="D142">
+        <v>5</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>38</v>
+      </c>
+      <c r="B143">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="10"/>
+        <v>17</v>
+      </c>
+      <c r="D143">
+        <v>3</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <f t="shared" si="8"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>39</v>
+      </c>
+      <c r="B144">
+        <v>6</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="D144">
+        <v>4</v>
+      </c>
+      <c r="E144">
+        <v>4</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>53</v>
+      </c>
+      <c r="B145">
+        <v>6</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="10"/>
+        <v>19</v>
+      </c>
+      <c r="D145">
+        <v>5</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>13</v>
+      </c>
+      <c r="B146">
+        <v>6</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="D146">
+        <v>3</v>
+      </c>
+      <c r="E146">
+        <v>2</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="8"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>20</v>
+      </c>
+      <c r="B147">
+        <v>6</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="10"/>
+        <v>21</v>
+      </c>
+      <c r="D147">
+        <v>4</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>24</v>
+      </c>
+      <c r="B148">
+        <v>6</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="10"/>
+        <v>22</v>
+      </c>
+      <c r="D148">
+        <v>4</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>52</v>
+      </c>
+      <c r="B149">
+        <v>6</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="10"/>
+        <v>23</v>
+      </c>
+      <c r="D149">
+        <v>4</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>55</v>
+      </c>
+      <c r="B150">
+        <v>6</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="D150">
+        <v>5</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>56</v>
+      </c>
+      <c r="B151">
+        <v>6</v>
+      </c>
+      <c r="C151">
+        <f t="shared" si="10"/>
         <v>25</v>
       </c>
-      <c r="C127" t="s">
-        <v>26</v>
-      </c>
-      <c r="D127" t="s">
-        <v>31</v>
-      </c>
-      <c r="E127" t="s">
+      <c r="D151">
+        <v>4</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>0</v>
+      </c>
+      <c r="B152" t="s">
+        <v>25</v>
+      </c>
+      <c r="C152" t="s">
+        <v>26</v>
+      </c>
+      <c r="D152" t="s">
+        <v>31</v>
+      </c>
+      <c r="E152" t="s">
         <v>32</v>
       </c>
-      <c r="F127" t="s">
+      <c r="F152" t="s">
         <v>33</v>
       </c>
-      <c r="G127" t="s">
+      <c r="G152" t="s">
         <v>34</v>
       </c>
-      <c r="H127" t="s">
+      <c r="H152" t="s">
         <v>46</v>
       </c>
-      <c r="I127" t="s">
+      <c r="I152" t="s">
         <v>45</v>
       </c>
-      <c r="J127" t="s">
+      <c r="J152" t="s">
         <v>27</v>
       </c>
-      <c r="K127" t="s">
+      <c r="K152" t="s">
         <v>28</v>
       </c>
-      <c r="L127" t="s">
+      <c r="L152" t="s">
         <v>29</v>
       </c>
-      <c r="M127" t="s">
+      <c r="M152" t="s">
         <v>30</v>
       </c>
-      <c r="N127" t="s">
+      <c r="N152" t="s">
         <v>40</v>
       </c>
-      <c r="O127" t="s">
+      <c r="O152" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>